<commit_message>
Adding new link to scraping
</commit_message>
<xml_diff>
--- a/dataSet/cleanData/bd.xlsx
+++ b/dataSet/cleanData/bd.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E313"/>
+  <dimension ref="A1:E314"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6282,16 +6282,16 @@
         </is>
       </c>
       <c r="B308" t="n">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C308" t="n">
-        <v>70</v>
+        <v>151</v>
       </c>
       <c r="D308" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E308" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="309">
@@ -6301,16 +6301,16 @@
         </is>
       </c>
       <c r="B309" t="n">
+        <v>26</v>
+      </c>
+      <c r="C309" t="n">
+        <v>86</v>
+      </c>
+      <c r="D309" t="n">
+        <v>1</v>
+      </c>
+      <c r="E309" t="n">
         <v>22</v>
-      </c>
-      <c r="C309" t="n">
-        <v>70</v>
-      </c>
-      <c r="D309" t="n">
-        <v>1</v>
-      </c>
-      <c r="E309" t="n">
-        <v>23</v>
       </c>
     </row>
     <row r="310">
@@ -6320,16 +6320,16 @@
         </is>
       </c>
       <c r="B310" t="n">
+        <v>27</v>
+      </c>
+      <c r="C310" t="n">
+        <v>90</v>
+      </c>
+      <c r="D310" t="n">
+        <v>1</v>
+      </c>
+      <c r="E310" t="n">
         <v>22</v>
-      </c>
-      <c r="C310" t="n">
-        <v>70</v>
-      </c>
-      <c r="D310" t="n">
-        <v>1</v>
-      </c>
-      <c r="E310" t="n">
-        <v>23</v>
       </c>
     </row>
     <row r="311">
@@ -6339,16 +6339,16 @@
         </is>
       </c>
       <c r="B311" t="n">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="C311" t="n">
-        <v>70</v>
+        <v>168</v>
       </c>
       <c r="D311" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E311" t="n">
-        <v>23</v>
+        <v>154</v>
       </c>
     </row>
     <row r="312">
@@ -6358,16 +6358,16 @@
         </is>
       </c>
       <c r="B312" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C312" t="n">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D312" t="n">
         <v>1</v>
       </c>
       <c r="E312" t="n">
-        <v>23</v>
+        <v>102</v>
       </c>
     </row>
     <row r="313">
@@ -6377,16 +6377,35 @@
         </is>
       </c>
       <c r="B313" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C313" t="n">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D313" t="n">
         <v>1</v>
       </c>
       <c r="E313" t="n">
-        <v>23</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>11.01.2021</t>
+        </is>
+      </c>
+      <c r="B314" t="n">
+        <v>6</v>
+      </c>
+      <c r="C314" t="n">
+        <v>43</v>
+      </c>
+      <c r="D314" t="n">
+        <v>3</v>
+      </c>
+      <c r="E314" t="n">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Starting to create a DL model
</commit_message>
<xml_diff>
--- a/dataSet/cleanData/bd.xlsx
+++ b/dataSet/cleanData/bd.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E314"/>
+  <dimension ref="A1:E317"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6408,6 +6408,63 @@
         <v>111</v>
       </c>
     </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>12.01.2021</t>
+        </is>
+      </c>
+      <c r="B315" t="n">
+        <v>14</v>
+      </c>
+      <c r="C315" t="n">
+        <v>79</v>
+      </c>
+      <c r="D315" t="n">
+        <v>2</v>
+      </c>
+      <c r="E315" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>13.01.2021</t>
+        </is>
+      </c>
+      <c r="B316" t="n">
+        <v>21</v>
+      </c>
+      <c r="C316" t="n">
+        <v>86</v>
+      </c>
+      <c r="D316" t="n">
+        <v>2</v>
+      </c>
+      <c r="E316" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>14.01.2021</t>
+        </is>
+      </c>
+      <c r="B317" t="n">
+        <v>15</v>
+      </c>
+      <c r="C317" t="n">
+        <v>69</v>
+      </c>
+      <c r="D317" t="n">
+        <v>2</v>
+      </c>
+      <c r="E317" t="n">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>